<commit_message>
Edits to Winkler data file from KN207-1 QL-1
</commit_message>
<xml_diff>
--- a/PHORCYS/data/processed/KN207_1/KN207data_Winklers_oxygen.xlsx
+++ b/PHORCYS/data/processed/KN207_1/KN207data_Winklers_oxygen.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcollins/Code/DO_Instruments/PHORCYS/data/processed/KN207_1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="33660" yWindow="2160" windowWidth="25600" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KN207data_Winklers_oxygen.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Data relevant for PHORCYS" sheetId="2" r:id="rId2"/>
     <sheet name="Usefully distilled!" sheetId="3" r:id="rId3"/>
-    <sheet name="Linear Regression" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="357">
   <si>
     <t>Determination start</t>
   </si>
@@ -1093,105 +1100,6 @@
   </si>
   <si>
     <t>Date/time</t>
-  </si>
-  <si>
-    <t>Standard Residuals</t>
-  </si>
-  <si>
-    <t>Residual</t>
-  </si>
-  <si>
-    <t>Predicted Y</t>
-  </si>
-  <si>
-    <t>Observation</t>
-  </si>
-  <si>
-    <t>Residuals</t>
-  </si>
-  <si>
-    <t>UCL - Upper value of a reliable interval (UCL)</t>
-  </si>
-  <si>
-    <t>LCL - Lower value of a reliable interval (LCL)</t>
-  </si>
-  <si>
-    <t>T (2%)</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Intercept</t>
-  </si>
-  <si>
-    <t>H0 (2%) rejected?</t>
-  </si>
-  <si>
-    <t>p-level</t>
-  </si>
-  <si>
-    <t>t Stat</t>
-  </si>
-  <si>
-    <t>UCL</t>
-  </si>
-  <si>
-    <t>LCL</t>
-  </si>
-  <si>
-    <t>Standard Error</t>
-  </si>
-  <si>
-    <t>Coefficients</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Regression</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>d.f.</t>
-  </si>
-  <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
-    <t>A = 199763.8744 - 5.0425 * B</t>
-  </si>
-  <si>
-    <t>Total number of observations</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Adjusted R Square</t>
-  </si>
-  <si>
-    <t>R Square</t>
-  </si>
-  <si>
-    <t>Regression Statistics</t>
-  </si>
-  <si>
-    <t>Linear Regression</t>
   </si>
 </sst>
 </file>
@@ -1201,9 +1109,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ hh:mm"/>
-    <numFmt numFmtId="166" formatCode="#,##0.#####"/>
+    <numFmt numFmtId="170" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1233,22 +1141,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1261,14 +1155,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="9"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1277,43 +1165,44 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="medium">
-        <color indexed="8"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="114">
+  <cellStyleXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1428,42 +1317,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="109"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="109" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="109" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="109" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="109" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="109" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="109" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="109" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="4" xfId="109" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="109" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="109" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="109" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="109" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="109" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="109" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="109" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="109" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="109" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="109"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="114">
+  <cellStyles count="134">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1520,6 +1406,16 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1576,11 +1472,26 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="109"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3086,11 +2997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111235736"/>
-        <c:axId val="-2111232776"/>
+        <c:axId val="-1955644752"/>
+        <c:axId val="-1951925344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111235736"/>
+        <c:axId val="-1955644752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250.0"/>
@@ -3101,12 +3012,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111232776"/>
+        <c:crossAx val="-1951925344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111232776"/>
+        <c:axId val="-1951925344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3117,7 +3028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111235736"/>
+        <c:crossAx val="-1955644752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3266,11 +3177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111204584"/>
-        <c:axId val="-2111201560"/>
+        <c:axId val="-1951903584"/>
+        <c:axId val="-1951901264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111204584"/>
+        <c:axId val="-1951903584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3280,12 +3191,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111201560"/>
+        <c:crossAx val="-1951901264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111201560"/>
+        <c:axId val="-1951901264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3296,142 +3207,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111204584"/>
+        <c:crossAx val="-1951903584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="47625">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>('Usefully distilled!'!$B$9,'Usefully distilled!'!$B$27)</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy\ h:mm</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>41026.70138888889</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41023.75208333333</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>('Usefully distilled!'!$G$9,'Usefully distilled!'!$G$27)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>260.12217</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>274.99395</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-2111159640"/>
-        <c:axId val="-2111156616"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="-2111159640"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy\ h:mm" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111156616"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="-2111156616"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111159640"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3503,41 +3285,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3874,7 +3621,7 @@
       <selection activeCell="E233" sqref="E233:E244"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="23.5" customWidth="1"/>
@@ -3882,7 +3629,7 @@
     <col min="10" max="10" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3932,7 +3679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3940,7 +3687,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3992,7 +3739,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -4047,7 +3794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4102,7 +3849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -4157,7 +3904,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -4212,7 +3959,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -4267,7 +4014,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -4322,7 +4069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -4377,7 +4124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4432,7 +4179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -4487,7 +4234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -4542,7 +4289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -4597,7 +4344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -4652,7 +4399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -4701,7 +4448,7 @@
         <v>4.3132599999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -4750,7 +4497,7 @@
         <v>4.3132599999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -4805,7 +4552,7 @@
         <v>55.1</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -4860,7 +4607,7 @@
         <v>55.1</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -4915,7 +4662,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -4970,7 +4717,7 @@
         <v>41.2</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -5025,7 +4772,7 @@
         <v>31.3</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -5080,7 +4827,7 @@
         <v>31.3</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -5135,7 +4882,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -5190,7 +4937,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -5245,7 +4992,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -5300,7 +5047,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -5355,7 +5102,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -5410,7 +5157,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -5465,7 +5212,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -5520,7 +5267,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -5575,7 +5322,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -5630,7 +5377,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -5685,7 +5432,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -5740,7 +5487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -5795,7 +5542,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -5850,7 +5597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -5905,7 +5652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -5960,7 +5707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -6015,7 +5762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -6070,7 +5817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -6125,7 +5872,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -6180,7 +5927,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>73</v>
       </c>
@@ -6235,7 +5982,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -6290,7 +6037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -6345,7 +6092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -6400,7 +6147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -6455,7 +6202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -6510,7 +6257,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -6565,7 +6312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>84</v>
       </c>
@@ -6620,7 +6367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -6675,7 +6422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>87</v>
       </c>
@@ -6730,7 +6477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -6785,7 +6532,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>91</v>
       </c>
@@ -6840,7 +6587,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>92</v>
       </c>
@@ -6895,7 +6642,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>94</v>
       </c>
@@ -6950,7 +6697,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>95</v>
       </c>
@@ -7005,7 +6752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>97</v>
       </c>
@@ -7060,7 +6807,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>98</v>
       </c>
@@ -7115,7 +6862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>100</v>
       </c>
@@ -7170,7 +6917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>101</v>
       </c>
@@ -7225,7 +6972,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>103</v>
       </c>
@@ -7280,7 +7027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>104</v>
       </c>
@@ -7335,7 +7082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>106</v>
       </c>
@@ -7390,7 +7137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>107</v>
       </c>
@@ -7445,7 +7192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>109</v>
       </c>
@@ -7500,7 +7247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -7555,7 +7302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -7610,7 +7357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>113</v>
       </c>
@@ -7665,7 +7412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>115</v>
       </c>
@@ -7720,7 +7467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>116</v>
       </c>
@@ -7775,7 +7522,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>118</v>
       </c>
@@ -7830,7 +7577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>119</v>
       </c>
@@ -7885,7 +7632,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>121</v>
       </c>
@@ -7940,7 +7687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>122</v>
       </c>
@@ -7995,7 +7742,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>124</v>
       </c>
@@ -8050,7 +7797,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>125</v>
       </c>
@@ -8105,7 +7852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>127</v>
       </c>
@@ -8160,7 +7907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>128</v>
       </c>
@@ -8215,7 +7962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>130</v>
       </c>
@@ -8270,7 +8017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>131</v>
       </c>
@@ -8325,7 +8072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>133</v>
       </c>
@@ -8380,7 +8127,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>134</v>
       </c>
@@ -8435,7 +8182,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>136</v>
       </c>
@@ -8490,7 +8237,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>137</v>
       </c>
@@ -8545,7 +8292,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>139</v>
       </c>
@@ -8600,7 +8347,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>140</v>
       </c>
@@ -8655,7 +8402,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>142</v>
       </c>
@@ -8710,7 +8457,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>143</v>
       </c>
@@ -8765,7 +8512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>146</v>
       </c>
@@ -8820,7 +8567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>147</v>
       </c>
@@ -8875,7 +8622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>149</v>
       </c>
@@ -8930,7 +8677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>150</v>
       </c>
@@ -8985,7 +8732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>152</v>
       </c>
@@ -9040,7 +8787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:17">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>153</v>
       </c>
@@ -9095,7 +8842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>155</v>
       </c>
@@ -9150,7 +8897,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>156</v>
       </c>
@@ -9205,7 +8952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>158</v>
       </c>
@@ -9260,7 +9007,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>159</v>
       </c>
@@ -9315,7 +9062,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>161</v>
       </c>
@@ -9370,7 +9117,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>162</v>
       </c>
@@ -9428,7 +9175,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>166</v>
       </c>
@@ -9486,7 +9233,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:18">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>167</v>
       </c>
@@ -9544,7 +9291,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="105" spans="1:18">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>169</v>
       </c>
@@ -9602,7 +9349,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="106" spans="1:18">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>170</v>
       </c>
@@ -9660,7 +9407,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:18">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>172</v>
       </c>
@@ -9718,7 +9465,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="108" spans="1:18">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>173</v>
       </c>
@@ -9776,7 +9523,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="109" spans="1:18">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>175</v>
       </c>
@@ -9834,7 +9581,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="110" spans="1:18">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>176</v>
       </c>
@@ -9892,7 +9639,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>178</v>
       </c>
@@ -9950,7 +9697,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="112" spans="1:18">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>179</v>
       </c>
@@ -10008,7 +9755,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="113" spans="1:18">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>181</v>
       </c>
@@ -10066,7 +9813,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="114" spans="1:18">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>182</v>
       </c>
@@ -10121,7 +9868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:18">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>184</v>
       </c>
@@ -10176,7 +9923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:18">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>185</v>
       </c>
@@ -10231,7 +9978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:18">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>187</v>
       </c>
@@ -10286,7 +10033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:18">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>188</v>
       </c>
@@ -10341,7 +10088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:18">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>190</v>
       </c>
@@ -10396,7 +10143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:18">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>191</v>
       </c>
@@ -10451,7 +10198,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:18">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>193</v>
       </c>
@@ -10506,7 +10253,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:18">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>194</v>
       </c>
@@ -10561,7 +10308,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="123" spans="1:18">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>196</v>
       </c>
@@ -10616,7 +10363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="124" spans="1:18">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>197</v>
       </c>
@@ -10671,7 +10418,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="125" spans="1:18">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>199</v>
       </c>
@@ -10726,7 +10473,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="1:18">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>200</v>
       </c>
@@ -10781,7 +10528,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="127" spans="1:18">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>202</v>
       </c>
@@ -10839,7 +10586,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="128" spans="1:18">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>204</v>
       </c>
@@ -10894,7 +10641,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="129" spans="1:18">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>206</v>
       </c>
@@ -10949,7 +10696,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="130" spans="1:18">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>207</v>
       </c>
@@ -11004,7 +10751,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="131" spans="1:18">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>209</v>
       </c>
@@ -11059,7 +10806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:18">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>210</v>
       </c>
@@ -11114,7 +10861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="133" spans="1:18">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>212</v>
       </c>
@@ -11169,7 +10916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="134" spans="1:18">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>213</v>
       </c>
@@ -11224,7 +10971,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="135" spans="1:18">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>215</v>
       </c>
@@ -11279,7 +11026,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="136" spans="1:18">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>216</v>
       </c>
@@ -11337,7 +11084,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="137" spans="1:18">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>219</v>
       </c>
@@ -11395,7 +11142,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="138" spans="1:18">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>222</v>
       </c>
@@ -11450,7 +11197,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="139" spans="1:18">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>225</v>
       </c>
@@ -11505,7 +11252,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="140" spans="1:18">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>226</v>
       </c>
@@ -11560,7 +11307,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="141" spans="1:18">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>228</v>
       </c>
@@ -11615,7 +11362,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="142" spans="1:18">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>230</v>
       </c>
@@ -11670,7 +11417,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="143" spans="1:18">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>232</v>
       </c>
@@ -11725,7 +11472,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="144" spans="1:18">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>233</v>
       </c>
@@ -11780,7 +11527,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="145" spans="1:17">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>235</v>
       </c>
@@ -11835,7 +11582,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="146" spans="1:17">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>236</v>
       </c>
@@ -11890,7 +11637,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="147" spans="1:17">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>239</v>
       </c>
@@ -11945,7 +11692,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="148" spans="1:17">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>240</v>
       </c>
@@ -12000,7 +11747,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="149" spans="1:17">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>241</v>
       </c>
@@ -12055,7 +11802,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="150" spans="1:17">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>243</v>
       </c>
@@ -12110,7 +11857,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="151" spans="1:17">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>244</v>
       </c>
@@ -12165,7 +11912,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="152" spans="1:17">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>245</v>
       </c>
@@ -12220,7 +11967,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="153" spans="1:17">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>247</v>
       </c>
@@ -12275,7 +12022,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="154" spans="1:17">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>248</v>
       </c>
@@ -12330,7 +12077,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="155" spans="1:17">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>249</v>
       </c>
@@ -12385,7 +12132,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="156" spans="1:17">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>251</v>
       </c>
@@ -12440,7 +12187,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="157" spans="1:17">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>252</v>
       </c>
@@ -12495,7 +12242,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="158" spans="1:17">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>254</v>
       </c>
@@ -12550,7 +12297,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="159" spans="1:17">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>255</v>
       </c>
@@ -12605,7 +12352,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="160" spans="1:17">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>257</v>
       </c>
@@ -12660,7 +12407,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="161" spans="1:18">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>258</v>
       </c>
@@ -12715,7 +12462,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="1:18">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>259</v>
       </c>
@@ -12773,7 +12520,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="163" spans="1:18">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>261</v>
       </c>
@@ -12828,7 +12575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="164" spans="1:18">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>262</v>
       </c>
@@ -12883,7 +12630,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:18">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>263</v>
       </c>
@@ -12938,7 +12685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:18">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>264</v>
       </c>
@@ -12993,7 +12740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="167" spans="1:18">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>265</v>
       </c>
@@ -13048,7 +12795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="168" spans="1:18">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>266</v>
       </c>
@@ -13103,7 +12850,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="169" spans="1:18">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>267</v>
       </c>
@@ -13158,7 +12905,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="170" spans="1:18">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>268</v>
       </c>
@@ -13213,7 +12960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="171" spans="1:18">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>269</v>
       </c>
@@ -13268,7 +13015,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="172" spans="1:18">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>270</v>
       </c>
@@ -13323,7 +13070,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="173" spans="1:18">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>271</v>
       </c>
@@ -13378,7 +13125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:18">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>272</v>
       </c>
@@ -13433,7 +13180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="1:18">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>273</v>
       </c>
@@ -13488,7 +13235,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="176" spans="1:18">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>274</v>
       </c>
@@ -13543,7 +13290,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="177" spans="1:17">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>275</v>
       </c>
@@ -13598,7 +13345,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="178" spans="1:17">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>276</v>
       </c>
@@ -13653,7 +13400,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="179" spans="1:17">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>277</v>
       </c>
@@ -13708,7 +13455,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="180" spans="1:17">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>278</v>
       </c>
@@ -13763,7 +13510,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="181" spans="1:17">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>279</v>
       </c>
@@ -13818,7 +13565,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="182" spans="1:17">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>280</v>
       </c>
@@ -13873,7 +13620,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="183" spans="1:17">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>281</v>
       </c>
@@ -13928,7 +13675,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="184" spans="1:17">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>282</v>
       </c>
@@ -13983,7 +13730,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="185" spans="1:17">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>283</v>
       </c>
@@ -14038,7 +13785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:17">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>284</v>
       </c>
@@ -14093,7 +13840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:17">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>285</v>
       </c>
@@ -14148,7 +13895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="1:17">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>286</v>
       </c>
@@ -14203,7 +13950,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="1:17">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>287</v>
       </c>
@@ -14258,7 +14005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="190" spans="1:17">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>288</v>
       </c>
@@ -14313,7 +14060,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:17">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>289</v>
       </c>
@@ -14368,7 +14115,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="192" spans="1:17">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>290</v>
       </c>
@@ -14423,7 +14170,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="193" spans="1:17">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>291</v>
       </c>
@@ -14478,7 +14225,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="194" spans="1:17">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>292</v>
       </c>
@@ -14533,7 +14280,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="195" spans="1:17">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>293</v>
       </c>
@@ -14588,7 +14335,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="196" spans="1:17">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>294</v>
       </c>
@@ -14643,7 +14390,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="197" spans="1:17">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>295</v>
       </c>
@@ -14698,7 +14445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="1:17">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>296</v>
       </c>
@@ -14753,7 +14500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:17">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>297</v>
       </c>
@@ -14808,7 +14555,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="200" spans="1:17">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>299</v>
       </c>
@@ -14863,7 +14610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="201" spans="1:17">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>300</v>
       </c>
@@ -14918,7 +14665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="202" spans="1:17">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>301</v>
       </c>
@@ -14973,7 +14720,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="203" spans="1:17">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>302</v>
       </c>
@@ -15028,7 +14775,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="204" spans="1:17">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>303</v>
       </c>
@@ -15083,7 +14830,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="205" spans="1:17">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>304</v>
       </c>
@@ -15138,7 +14885,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="206" spans="1:17">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>305</v>
       </c>
@@ -15193,7 +14940,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="207" spans="1:17">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>306</v>
       </c>
@@ -15248,7 +14995,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="208" spans="1:17">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>308</v>
       </c>
@@ -15303,7 +15050,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:18">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>309</v>
       </c>
@@ -15358,7 +15105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:18">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>310</v>
       </c>
@@ -15413,7 +15160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:18">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>311</v>
       </c>
@@ -15468,7 +15215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:18">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>312</v>
       </c>
@@ -15523,7 +15270,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="213" spans="1:18">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>313</v>
       </c>
@@ -15578,7 +15325,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="214" spans="1:18">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>314</v>
       </c>
@@ -15633,7 +15380,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="215" spans="1:18">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>315</v>
       </c>
@@ -15688,7 +15435,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="216" spans="1:18">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>316</v>
       </c>
@@ -15743,7 +15490,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="217" spans="1:18">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>317</v>
       </c>
@@ -15798,7 +15545,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="218" spans="1:18">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>318</v>
       </c>
@@ -15853,7 +15600,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="219" spans="1:18">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>319</v>
       </c>
@@ -15908,7 +15655,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="220" spans="1:18">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>320</v>
       </c>
@@ -15966,7 +15713,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="221" spans="1:18">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>322</v>
       </c>
@@ -16021,7 +15768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:18">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>323</v>
       </c>
@@ -16076,7 +15823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:18">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>324</v>
       </c>
@@ -16131,7 +15878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:18">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>325</v>
       </c>
@@ -16186,7 +15933,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="225" spans="1:17">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>326</v>
       </c>
@@ -16241,7 +15988,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="226" spans="1:17">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>327</v>
       </c>
@@ -16296,7 +16043,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="227" spans="1:17">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>328</v>
       </c>
@@ -16351,7 +16098,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="228" spans="1:17">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>329</v>
       </c>
@@ -16406,7 +16153,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="229" spans="1:17">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>330</v>
       </c>
@@ -16461,7 +16208,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="230" spans="1:17">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>331</v>
       </c>
@@ -16516,7 +16263,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="231" spans="1:17">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>332</v>
       </c>
@@ -16571,7 +16318,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="232" spans="1:17">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>333</v>
       </c>
@@ -16626,7 +16373,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="233" spans="1:17">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>334</v>
       </c>
@@ -16681,7 +16428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:17">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>335</v>
       </c>
@@ -16736,7 +16483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:17">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>336</v>
       </c>
@@ -16791,7 +16538,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:17">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>337</v>
       </c>
@@ -16846,7 +16593,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="237" spans="1:17">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>338</v>
       </c>
@@ -16901,7 +16648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="238" spans="1:17">
+    <row r="238" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>339</v>
       </c>
@@ -16956,7 +16703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="239" spans="1:17">
+    <row r="239" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>340</v>
       </c>
@@ -17011,7 +16758,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="240" spans="1:17">
+    <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>341</v>
       </c>
@@ -17066,7 +16813,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="241" spans="1:17">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>342</v>
       </c>
@@ -17121,7 +16868,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="242" spans="1:17">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>343</v>
       </c>
@@ -17176,7 +16923,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="243" spans="1:17">
+    <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>344</v>
       </c>
@@ -17231,7 +16978,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="244" spans="1:17">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>345</v>
       </c>
@@ -17290,11 +17037,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -17303,10 +17045,10 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I28"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
@@ -17315,7 +17057,7 @@
     <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -17350,7 +17092,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>45</v>
       </c>
@@ -17387,7 +17129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>45</v>
       </c>
@@ -17424,7 +17166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>45</v>
       </c>
@@ -17461,7 +17203,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>45</v>
       </c>
@@ -17498,7 +17240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>45</v>
       </c>
@@ -17535,7 +17277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>45</v>
       </c>
@@ -17572,7 +17314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>45</v>
       </c>
@@ -17609,7 +17351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>45</v>
       </c>
@@ -17646,7 +17388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>999</v>
       </c>
@@ -17683,7 +17425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>999</v>
       </c>
@@ -17720,7 +17462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>999</v>
       </c>
@@ -17757,7 +17499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>999</v>
       </c>
@@ -17794,7 +17536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>999</v>
       </c>
@@ -17831,7 +17573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>999</v>
       </c>
@@ -17868,7 +17610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>999</v>
       </c>
@@ -17905,7 +17647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>999</v>
       </c>
@@ -17942,7 +17684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>999</v>
       </c>
@@ -17979,7 +17721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>45</v>
       </c>
@@ -18016,7 +17758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>45</v>
       </c>
@@ -18053,7 +17795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>45</v>
       </c>
@@ -18090,7 +17832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>45</v>
       </c>
@@ -18127,7 +17869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>45</v>
       </c>
@@ -18164,7 +17906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>45</v>
       </c>
@@ -18201,7 +17943,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>26</v>
       </c>
@@ -18241,7 +17983,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -18281,7 +18023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -18321,7 +18063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -18364,23 +18106,18 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
@@ -18390,7 +18127,7 @@
     <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -18419,7 +18156,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18433,7 +18170,7 @@
         <v>260.09983999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18447,7 +18184,7 @@
         <v>260.50178</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18461,7 +18198,7 @@
         <v>259.83187999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18475,7 +18212,7 @@
         <v>260.94837999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18489,7 +18226,7 @@
         <v>260.41246000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18503,7 +18240,7 @@
         <v>259.87654000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18517,7 +18254,7 @@
         <v>259.65323999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="4">
         <v>41026.701388888891</v>
       </c>
@@ -18530,20 +18267,8 @@
       <c r="E9">
         <v>259.65323999999998</v>
       </c>
-      <c r="G9">
-        <f>AVERAGE(E2:E9)</f>
-        <v>260.12216999999998</v>
-      </c>
-      <c r="H9">
-        <f>STDEV(E2:E9)</f>
-        <v>0.46227491820344668</v>
-      </c>
-      <c r="I9">
-        <f>CONFIDENCE(0.05,H9,8)</f>
-        <v>0.32033428851954554</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>999</v>
       </c>
@@ -18560,7 +18285,7 @@
         <v>273.18521999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>999</v>
       </c>
@@ -18577,7 +18302,7 @@
         <v>273.36386000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>999</v>
       </c>
@@ -18594,7 +18319,7 @@
         <v>273.89978000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>999</v>
       </c>
@@ -18611,7 +18336,7 @@
         <v>273.22987999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>999</v>
       </c>
@@ -18628,7 +18353,7 @@
         <v>273.00658000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>999</v>
       </c>
@@ -18645,7 +18370,7 @@
         <v>274.30172000000005</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>999</v>
       </c>
@@ -18662,7 +18387,7 @@
         <v>272.51532000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>999</v>
       </c>
@@ -18679,7 +18404,7 @@
         <v>273.05124000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>999</v>
       </c>
@@ -18696,7 +18421,7 @@
         <v>273.40852000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>45</v>
       </c>
@@ -18713,7 +18438,7 @@
         <v>292.92493999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>45</v>
       </c>
@@ -18730,7 +18455,7 @@
         <v>293.14823999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>45</v>
       </c>
@@ -18747,7 +18472,7 @@
         <v>293.10358000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>45</v>
       </c>
@@ -18764,7 +18489,7 @@
         <v>293.77348000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>45</v>
       </c>
@@ -18781,7 +18506,7 @@
         <v>292.88027999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>45</v>
       </c>
@@ -18798,7 +18523,7 @@
         <v>293.50552000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>26</v>
       </c>
@@ -18818,7 +18543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -18838,7 +18563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -18857,20 +18582,8 @@
       <c r="F27">
         <v>30</v>
       </c>
-      <c r="G27">
-        <f>AVERAGE(E27:E28)</f>
-        <v>274.99395000000004</v>
-      </c>
-      <c r="H27">
-        <f>STDEV(E27:E28)</f>
-        <v>0.34737327732567103</v>
-      </c>
-      <c r="I27">
-        <f>CONFIDENCE(0.05,H27,2)</f>
-        <v>0.48142595352252859</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -18890,610 +18603,213 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
-      <c r="C33" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D33" s="6">
-        <v>260.09983999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4">
-      <c r="C34" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D34" s="6">
-        <v>260.50178</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4">
-      <c r="C35" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D35" s="6">
-        <v>259.83187999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4">
-      <c r="C36" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D36" s="6">
-        <v>260.94837999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4">
-      <c r="C37" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D37" s="6">
-        <v>260.41246000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4">
-      <c r="C38" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D38" s="6">
-        <v>259.87654000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4">
-      <c r="C39" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D39" s="6">
-        <v>259.65323999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4">
-      <c r="C40" s="5">
-        <v>41026.701388888891</v>
-      </c>
-      <c r="D40" s="6">
-        <v>259.65323999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4">
-      <c r="C41" s="5">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C33" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D33" t="s">
+        <v>237</v>
+      </c>
+      <c r="E33">
+        <v>8.7413765100000003</v>
+      </c>
+      <c r="F33">
+        <v>273.18521999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C34" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D34" t="s">
+        <v>237</v>
+      </c>
+      <c r="E34">
+        <v>8.7470926300000009</v>
+      </c>
+      <c r="F34">
+        <v>273.36386000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D35" t="s">
+        <v>237</v>
+      </c>
+      <c r="E35">
+        <v>8.7642409899999993</v>
+      </c>
+      <c r="F35">
+        <v>273.89978000000002</v>
+      </c>
+      <c r="G35">
+        <f>AVERAGE(F33:F35)</f>
+        <v>273.48295333333334</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C36" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D36" t="s">
+        <v>242</v>
+      </c>
+      <c r="E36">
+        <v>8.7428055400000009</v>
+      </c>
+      <c r="F36">
+        <v>273.22987999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C37" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D37" t="s">
+        <v>242</v>
+      </c>
+      <c r="E37">
+        <v>8.7356603900000014</v>
+      </c>
+      <c r="F37">
+        <v>273.00658000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C38" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D38" t="s">
+        <v>242</v>
+      </c>
+      <c r="E38">
+        <v>8.7771022600000013</v>
+      </c>
+      <c r="F38">
+        <v>274.30172000000005</v>
+      </c>
+      <c r="G38">
+        <f>AVERAGE(F36:F38)</f>
+        <v>273.51272666666671</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C39" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D39" t="s">
+        <v>246</v>
+      </c>
+      <c r="E39">
+        <v>8.71994106</v>
+      </c>
+      <c r="F39">
+        <v>272.51532000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C40" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D40" t="s">
+        <v>246</v>
+      </c>
+      <c r="E40">
+        <v>8.7370894200000002</v>
+      </c>
+      <c r="F40">
+        <v>273.05124000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="4">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D41" t="s">
+        <v>246</v>
+      </c>
+      <c r="E41">
+        <v>8.7485216599999998</v>
+      </c>
+      <c r="F41">
+        <v>273.40852000000001</v>
+      </c>
+      <c r="G41">
+        <f>AVERAGE(F39:F41)</f>
+        <v>272.99169333333333</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C43" s="5">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D43">
+        <v>273.482953333333</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="array" ref="I43:I48">LINEST(D43:D47,C43:C47,1,1)</f>
+        <v>-0.57380296792753172</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C44" s="5">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D44">
+        <v>273.51272666666671</v>
+      </c>
+      <c r="I44" s="7">
+        <v>9.8143295281823473E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C45" s="5">
+        <v>41026.65347222222</v>
+      </c>
+      <c r="D45">
+        <v>272.99169333333333</v>
+      </c>
+      <c r="I45" s="7">
+        <v>0.9193169659994328</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C46" s="4">
         <v>41023.752083333333</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D46">
         <v>274.74832000000004</v>
       </c>
-    </row>
-    <row r="42" spans="3:4">
-      <c r="C42" s="5">
+      <c r="I46" s="7">
+        <v>34.182538276620946</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C47" s="4">
         <v>41023.752083333333</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D47">
         <v>275.23957999999999</v>
       </c>
+      <c r="I47" s="7">
+        <v>3.3259729565174778</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="I48" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="7"/>
-    <col min="7" max="7" width="6.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="13" thickBot="1">
-      <c r="A1" s="22" t="s">
-        <v>389</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-    </row>
-    <row r="3" spans="1:8" ht="13" thickBot="1">
-      <c r="A3" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0.9977236988172169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="17" t="s">
-        <v>387</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0.99545257918150853</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0.99488415157919707</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
-        <v>385</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0.44952125836829554</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="B8" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="13" thickBot="1">
-      <c r="A9" s="22" t="s">
-        <v>383</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:8" ht="13" thickBot="1">
-      <c r="A11" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="11" t="s">
-        <v>375</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>381</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>378</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="17" t="s">
-        <v>377</v>
-      </c>
-      <c r="B13" s="9">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>353.87174458941701</v>
-      </c>
-      <c r="D13" s="9">
-        <v>353.87174458941701</v>
-      </c>
-      <c r="E13" s="9">
-        <v>1751.2389882785885</v>
-      </c>
-      <c r="F13" s="9">
-        <v>1.171412966627372E-10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="17" t="s">
-        <v>358</v>
-      </c>
-      <c r="B14" s="9">
-        <v>8</v>
-      </c>
-      <c r="C14" s="9">
-        <v>1.6165548938001275</v>
-      </c>
-      <c r="D14" s="9">
-        <v>0.20206936172501594</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="13" thickBot="1">
-      <c r="A15" s="21" t="s">
-        <v>376</v>
-      </c>
-      <c r="B15" s="20">
-        <v>9</v>
-      </c>
-      <c r="C15" s="20">
-        <v>355.48829948321713</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" ht="13" thickBot="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="11" t="s">
-        <v>375</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>374</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>369</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="B18" s="9">
-        <v>199763.87437616216</v>
-      </c>
-      <c r="C18" s="9">
-        <v>4767.2934810622064</v>
-      </c>
-      <c r="D18" s="9">
-        <v>185955.60213293505</v>
-      </c>
-      <c r="E18" s="9">
-        <v>213572.14661938927</v>
-      </c>
-      <c r="F18" s="9">
-        <v>41.902994890017247</v>
-      </c>
-      <c r="G18" s="9">
-        <v>1.1591771986729782E-10</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="B19" s="9">
-        <v>-5.0424682912465659</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0.12049540087854069</v>
-      </c>
-      <c r="D19" s="9">
-        <v>-5.3914783335267735</v>
-      </c>
-      <c r="E19" s="9">
-        <v>-4.6934582489663583</v>
-      </c>
-      <c r="F19" s="9">
-        <v>-41.847807090408139</v>
-      </c>
-      <c r="G19" s="9">
-        <v>1.171412966627372E-10</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="B20" s="15">
-        <v>2.8964594477096219</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="24" t="s">
-        <v>363</v>
-      </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-    </row>
-    <row r="22" spans="1:8" ht="13" thickBot="1">
-      <c r="A22" s="24" t="s">
-        <v>362</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" ht="13" thickBot="1">
-      <c r="A24" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>357</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="7">
-        <v>1</v>
-      </c>
-      <c r="B26" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C26" s="9">
-        <v>-2.233005092506346E-2</v>
-      </c>
-      <c r="D26" s="9">
-        <v>-5.2688488522815005E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="7">
-        <v>2</v>
-      </c>
-      <c r="B27" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C27" s="9">
-        <v>0.37960994907496115</v>
-      </c>
-      <c r="D27" s="9">
-        <v>0.89570214152814343</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="7">
-        <v>3</v>
-      </c>
-      <c r="B28" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C28" s="9">
-        <v>-0.29029005092502302</v>
-      </c>
-      <c r="D28" s="9">
-        <v>-0.68494890855665314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="7">
-        <v>4</v>
-      </c>
-      <c r="B29" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C29" s="9">
-        <v>0.8262099490749506</v>
-      </c>
-      <c r="D29" s="9">
-        <v>1.9494695082513411</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="7">
-        <v>5</v>
-      </c>
-      <c r="B30" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C30" s="9">
-        <v>0.29028994907497463</v>
-      </c>
-      <c r="D30" s="9">
-        <v>0.68494866818353062</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="7">
-        <v>6</v>
-      </c>
-      <c r="B31" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C31" s="9">
-        <v>-0.24563005092505819</v>
-      </c>
-      <c r="D31" s="9">
-        <v>-0.57957217188441379</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="7">
-        <v>7</v>
-      </c>
-      <c r="B32" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C32" s="9">
-        <v>-0.46893005092505291</v>
-      </c>
-      <c r="D32" s="9">
-        <v>-1.1064558552460126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="7">
-        <v>8</v>
-      </c>
-      <c r="B33" s="9">
-        <v>260.12217005092504</v>
-      </c>
-      <c r="C33" s="9">
-        <v>-0.46893005092505291</v>
-      </c>
-      <c r="D33" s="9">
-        <v>-1.1064558552460126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="7">
-        <v>9</v>
-      </c>
-      <c r="B34" s="9">
-        <v>274.99394979624196</v>
-      </c>
-      <c r="C34" s="9">
-        <v>-0.24562979624198533</v>
-      </c>
-      <c r="D34" s="9">
-        <v>-0.57957157095133949</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="13" thickBot="1">
-      <c r="A35" s="7">
-        <v>10</v>
-      </c>
-      <c r="B35" s="9">
-        <v>274.99394979624196</v>
-      </c>
-      <c r="C35" s="9">
-        <v>0.2456302037580258</v>
-      </c>
-      <c r="D35" s="9">
-        <v>0.57957253244423168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial commit Iselin November 2016 Winkler data
</commit_message>
<xml_diff>
--- a/PHORCYS/data/processed/KN207_1/KN207data_Winklers_oxygen.xlsx
+++ b/PHORCYS/data/processed/KN207_1/KN207data_Winklers_oxygen.xlsx
@@ -1109,7 +1109,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ hh:mm"/>
-    <numFmt numFmtId="170" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1344,7 +1344,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2997,11 +2997,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1955644752"/>
-        <c:axId val="-1951925344"/>
+        <c:axId val="1687060080"/>
+        <c:axId val="1686437664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1955644752"/>
+        <c:axId val="1687060080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250.0"/>
@@ -3012,12 +3012,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1951925344"/>
+        <c:crossAx val="1686437664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1951925344"/>
+        <c:axId val="1686437664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3028,7 +3028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1955644752"/>
+        <c:crossAx val="1687060080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3177,11 +3177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1951903584"/>
-        <c:axId val="-1951901264"/>
+        <c:axId val="1684597088"/>
+        <c:axId val="1684964960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1951903584"/>
+        <c:axId val="1684597088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3191,12 +3191,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1951901264"/>
+        <c:crossAx val="1684964960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1951901264"/>
+        <c:axId val="1684964960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3207,7 +3207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1951903584"/>
+        <c:crossAx val="1684597088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18113,8 +18113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18267,6 +18267,10 @@
       <c r="E9">
         <v>259.65323999999998</v>
       </c>
+      <c r="G9">
+        <f>AVERAGE(E2:E9)</f>
+        <v>260.12216999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">

</xml_diff>